<commit_message>
add script for depersonalization
</commit_message>
<xml_diff>
--- a/describe_normalized_x_train.xlsx
+++ b/describe_normalized_x_train.xlsx
@@ -1017,202 +1017,202 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5074983410749835</v>
+        <v>0.462043795620438</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5328467153284672</v>
+        <v>0.4854014598540146</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2700729927007299</v>
+        <v>0.2554744525547445</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5693430656934306</v>
+        <v>0.5182481751824818</v>
       </c>
       <c r="F3" t="n">
-        <v>0.08029197080291971</v>
+        <v>0.1021897810218978</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7036040145985401</v>
+        <v>0.7467669631750652</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7343677150609547</v>
+        <v>0.7336931200496971</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7374087591240875</v>
+        <v>0.7325086438724548</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4229851161247512</v>
+        <v>0.4254385832780359</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4311146103042851</v>
+        <v>0.4333354317807579</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6879919528831658</v>
+        <v>0.6969385472475346</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6665256926323772</v>
+        <v>0.6752470491091697</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2275995042005233</v>
+        <v>0.2049129702414374</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2869804856249069</v>
+        <v>0.01267405675935353</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1569866936751301</v>
+        <v>0.1437286223068514</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1981674173008231</v>
+        <v>0.1774106799846331</v>
       </c>
       <c r="R3" t="n">
-        <v>0.6624904673711733</v>
+        <v>0.6724588735156335</v>
       </c>
       <c r="S3" t="n">
-        <v>0.6369800889733511</v>
+        <v>0.6050479783482325</v>
       </c>
       <c r="T3" t="n">
-        <v>0.6113740274324216</v>
+        <v>0.6103404989171414</v>
       </c>
       <c r="U3" t="n">
-        <v>0.5419604932162151</v>
+        <v>0.5431357994144088</v>
       </c>
       <c r="V3" t="n">
-        <v>0.3227017877922354</v>
+        <v>0.353697238971755</v>
       </c>
       <c r="W3" t="n">
-        <v>0.4337983923126675</v>
+        <v>0.3949921463549847</v>
       </c>
       <c r="X3" t="n">
-        <v>0.4316788321167883</v>
+        <v>0.4659854014598541</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.6167883211678832</v>
+        <v>0.6385401459854015</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.6237623762376238</v>
+        <v>0.6387222663872226</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.2490283439188549</v>
+        <v>0.2338071456012293</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.2585268745852688</v>
+        <v>0.2047217153284671</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.6803434194025532</v>
+        <v>0.6689925721084279</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.6604116412393095</v>
+        <v>0.6545534287772939</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.7387213085920324</v>
+        <v>0.7540233928414387</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.7500225286113364</v>
+        <v>0.7396007387213086</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.7361479761114798</v>
+        <v>0.745686794956868</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.7174021234240212</v>
+        <v>0.7205540809555409</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.7400547445255473</v>
+        <v>0.7423357664233576</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.7379132674967798</v>
+        <v>0.7524259338772005</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.3941605839416059</v>
+        <v>0.4014598540145985</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.4583609820836098</v>
+        <v>0.458029197080292</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.3868613138686132</v>
+        <v>0.4233576642335766</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.343065693430657</v>
+        <v>0.364963503649635</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.3576642335766423</v>
+        <v>0.3795620437956204</v>
       </c>
       <c r="AP3" t="n">
         <v>0</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.1532846715328467</v>
+        <v>0.1313868613138686</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1970802919708029</v>
+        <v>0.2043795620437956</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.1970802919708029</v>
+        <v>0.2043795620437956</v>
       </c>
       <c r="AT3" t="n">
+        <v>0.072992700729927</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.072992700729927</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.072992700729927</v>
+      </c>
+      <c r="AW3" t="n">
         <v>0.08759124087591241</v>
       </c>
-      <c r="AU3" t="n">
-        <v>0.08759124087591241</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>0.08759124087591241</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>0.1094890510948905</v>
-      </c>
       <c r="AX3" t="n">
+        <v>0.05109489051094891</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0.06569343065693431</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0.05109489051094891</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0.05109489051094891</v>
+      </c>
+      <c r="BB3" t="n">
         <v>0.04379562043795621</v>
       </c>
-      <c r="AY3" t="n">
+      <c r="BC3" t="n">
+        <v>0.04379562043795621</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.04379562043795621</v>
+      </c>
+      <c r="BE3" t="n">
         <v>0.0583941605839416</v>
       </c>
-      <c r="AZ3" t="n">
-        <v>0.04379562043795621</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0.04379562043795621</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0.05109489051094891</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>0.05109489051094891</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>0.05109489051094891</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>0.04379562043795621</v>
-      </c>
       <c r="BF3" t="n">
-        <v>0.04379562043795621</v>
+        <v>0.0583941605839416</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.04379562043795621</v>
+        <v>0.0583941605839416</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.04379562043795621</v>
+        <v>0.0583941605839416</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.04379562043795621</v>
+        <v>0.0583941605839416</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.05109489051094891</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.05109489051094891</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.05109489051094891</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.05109489051094891</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.05109489051094891</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.072992700729927</v>
+        <v>0.06569343065693431</v>
       </c>
       <c r="BP3" t="n">
         <v>0.06569343065693431</v>
@@ -1227,7 +1227,7 @@
         <v>0.05109489051094891</v>
       </c>
       <c r="BT3" t="n">
-        <v>0.0583941605839416</v>
+        <v>0.05109489051094891</v>
       </c>
     </row>
     <row r="4">
@@ -1237,202 +1237,202 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3011481388278348</v>
+        <v>0.3461256811182618</v>
       </c>
       <c r="C4" t="n">
-        <v>0.500750831700448</v>
+        <v>0.4997852694768909</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2636249524379707</v>
+        <v>0.2689326935581176</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4969853299698476</v>
+        <v>0.5015005392792523</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2727419099081623</v>
+        <v>0.3040092764849821</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3058261131083288</v>
+        <v>0.2965072301990125</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3662921037558999</v>
+        <v>0.374112627417894</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3680033800567206</v>
+        <v>0.3737938413659845</v>
       </c>
       <c r="J4" t="n">
-        <v>0.179322493425861</v>
+        <v>0.1687738691158554</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1904223307840432</v>
+        <v>0.1810107455675833</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2407833194970583</v>
+        <v>0.2218866884584537</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2619700181569372</v>
+        <v>0.2386735989225567</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1560194975060461</v>
+        <v>0.1683819789862626</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1729320700641761</v>
+        <v>0.08503786694531396</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1334835579803631</v>
+        <v>0.1445811207769394</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2239660351989991</v>
+        <v>0.2285815737140521</v>
       </c>
       <c r="R4" t="n">
-        <v>0.198057063079844</v>
+        <v>0.1968223587002977</v>
       </c>
       <c r="S4" t="n">
-        <v>0.2064962980770886</v>
+        <v>0.2032568703546531</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2002476052071398</v>
+        <v>0.210620122106326</v>
       </c>
       <c r="U4" t="n">
-        <v>0.1765232742677893</v>
+        <v>0.1894416995281113</v>
       </c>
       <c r="V4" t="n">
-        <v>0.2108951447802487</v>
+        <v>0.2249185825300107</v>
       </c>
       <c r="W4" t="n">
-        <v>0.2085776019105534</v>
+        <v>0.2076489890720712</v>
       </c>
       <c r="X4" t="n">
-        <v>0.2337783305985598</v>
+        <v>0.245448149112929</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.2269521014073018</v>
+        <v>0.2386251679997726</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2356743958726239</v>
+        <v>0.2422653732954648</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2439117982194263</v>
+        <v>0.2130094680917154</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.1861739654153585</v>
+        <v>0.16711194210222</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.1856132821724688</v>
+        <v>0.2040565692171277</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1765806928950575</v>
+        <v>0.1978498581907108</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.2292453136923608</v>
+        <v>0.2217953502494493</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.2201029677253424</v>
+        <v>0.2180417856311708</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.1957050307048384</v>
+        <v>0.1978062577872582</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.2029788937262349</v>
+        <v>0.2064010581405945</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.1974570567500999</v>
+        <v>0.201141321674305</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.2121139465763503</v>
+        <v>0.2043834144943563</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.4904629300853346</v>
+        <v>0.4919925575506937</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.2335459322536829</v>
+        <v>0.2342493770603732</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.488818731927854</v>
+        <v>0.4959042207278343</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.4764753589761638</v>
+        <v>0.4831866100471024</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.4810715104811871</v>
+        <v>0.4870588027869559</v>
       </c>
       <c r="AP4" t="n">
         <v>0</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.3615837497346002</v>
+        <v>0.3390626839533289</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.3992532746632467</v>
+        <v>0.4047273252629636</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.3992532746632467</v>
+        <v>0.4047273252629636</v>
       </c>
       <c r="AT4" t="n">
+        <v>0.2610791094992419</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.2610791094992419</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>0.2610791094992419</v>
+      </c>
+      <c r="AW4" t="n">
         <v>0.283736947218425</v>
       </c>
-      <c r="AU4" t="n">
-        <v>0.283736947218425</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>0.283736947218425</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>0.313397701594211</v>
-      </c>
       <c r="AX4" t="n">
+        <v>0.2209993306887549</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.2486546022226944</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>0.2209993306887549</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.2209993306887549</v>
+      </c>
+      <c r="BB4" t="n">
         <v>0.2053910595269901</v>
       </c>
-      <c r="AY4" t="n">
+      <c r="BC4" t="n">
+        <v>0.2053910595269901</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0.2053910595269901</v>
+      </c>
+      <c r="BE4" t="n">
         <v>0.2353477826306845</v>
       </c>
-      <c r="AZ4" t="n">
-        <v>0.2053910595269901</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>0.2053910595269901</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>0.2209993306887549</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>0.2209993306887549</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>0.2209993306887549</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>0.2053910595269901</v>
-      </c>
       <c r="BF4" t="n">
-        <v>0.2053910595269901</v>
+        <v>0.2353477826306845</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.2053910595269901</v>
+        <v>0.2353477826306845</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.2053910595269901</v>
+        <v>0.2353477826306845</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.2053910595269901</v>
+        <v>0.2353477826306845</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.2209993306887549</v>
+        <v>0.2486546022226944</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.2209993306887549</v>
+        <v>0.2486546022226944</v>
       </c>
       <c r="BL4" t="n">
-        <v>0.2209993306887549</v>
+        <v>0.2486546022226944</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.2209993306887549</v>
+        <v>0.2486546022226944</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.2209993306887549</v>
+        <v>0.2486546022226944</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.2610791094992419</v>
+        <v>0.2486546022226944</v>
       </c>
       <c r="BP4" t="n">
         <v>0.2486546022226944</v>
@@ -1447,7 +1447,7 @@
         <v>0.2209993306887549</v>
       </c>
       <c r="BT4" t="n">
-        <v>0.2353477826306844</v>
+        <v>0.2209993306887549</v>
       </c>
     </row>
     <row r="5">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2181818181818182</v>
+        <v>0.1545454545454545</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1692,94 +1692,94 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7562500000000001</v>
+        <v>0.7942122186495176</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8691099476439791</v>
+        <v>0.8829787234042553</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8697916666666666</v>
+        <v>0.8736842105263157</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3431818181818182</v>
+        <v>0.3513636363636364</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3522813231783014</v>
+        <v>0.3529019173996812</v>
       </c>
       <c r="L6" t="n">
-        <v>0.654941891661564</v>
+        <v>0.6570995701056114</v>
       </c>
       <c r="M6" t="n">
-        <v>0.620594941900205</v>
+        <v>0.628844839371155</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1245283018867925</v>
+        <v>0.1</v>
       </c>
       <c r="O6" t="n">
-        <v>0.173469387755102</v>
+        <v>0.003536345776031434</v>
       </c>
       <c r="P6" t="n">
-        <v>0.08133971291866028</v>
+        <v>0.06763285024154589</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02127659574468085</v>
+        <v>0.01052631578947368</v>
       </c>
       <c r="R6" t="n">
-        <v>0.6194029850746269</v>
+        <v>0.6268656716417911</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5857988165680473</v>
+        <v>0.5561797752808989</v>
       </c>
       <c r="T6" t="n">
-        <v>0.5384615384615385</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="U6" t="n">
-        <v>0.4604519774011299</v>
+        <v>0.4632768361581921</v>
       </c>
       <c r="V6" t="n">
-        <v>0.177536231884058</v>
+        <v>0.2065217391304348</v>
       </c>
       <c r="W6" t="n">
-        <v>0.2995780590717299</v>
+        <v>0.270042194092827</v>
       </c>
       <c r="X6" t="n">
-        <v>0.28</v>
+        <v>0.32</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.5247524752475248</v>
+        <v>0.5643564356435643</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.07792207792207792</v>
+        <v>0.0736842105263158</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.1090909090909091</v>
+        <v>0.078125</v>
       </c>
       <c r="AC6" t="n">
         <v>0.6387665198237885</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.6137339055793991</v>
+        <v>0.6223175965665236</v>
       </c>
       <c r="AE6" t="n">
+        <v>0.7349397590361446</v>
+      </c>
+      <c r="AF6" t="n">
         <v>0.7228915662650602</v>
       </c>
-      <c r="AF6" t="n">
-        <v>0.728395061728395</v>
-      </c>
       <c r="AG6" t="n">
-        <v>0.7045454545454546</v>
+        <v>0.7159090909090909</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.6931818181818182</v>
+        <v>0.6818181818181819</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.7125</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.7058823529411764</v>
+        <v>0.7176470588235294</v>
       </c>
       <c r="AK6" t="n">
         <v>0</v>
@@ -1897,10 +1897,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5363636363636364</v>
+        <v>0.3818181818181818</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0.3333333333333333</v>
@@ -1912,94 +1912,94 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8125</v>
+        <v>0.842443729903537</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9005235602094241</v>
+        <v>0.9095744680851063</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9010416666666666</v>
+        <v>0.9052631578947368</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4454545454545455</v>
+        <v>0.4357</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4557673399020127</v>
+        <v>0.4463838684108614</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7346396399239953</v>
+        <v>0.738456609705134</v>
       </c>
       <c r="M7" t="n">
-        <v>0.7332406015037592</v>
+        <v>0.7328694463431304</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1849056603773585</v>
+        <v>0.1576923076923077</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2653061224489796</v>
+        <v>0.004911591355599214</v>
       </c>
       <c r="P7" t="n">
-        <v>0.1244019138755981</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.148936170212766</v>
+        <v>0.08421052631578947</v>
       </c>
       <c r="R7" t="n">
-        <v>0.7014925373134329</v>
+        <v>0.7164179104477612</v>
       </c>
       <c r="S7" t="n">
-        <v>0.6863905325443787</v>
+        <v>0.6573033707865168</v>
       </c>
       <c r="T7" t="n">
-        <v>0.6538461538461539</v>
+        <v>0.6593406593406594</v>
       </c>
       <c r="U7" t="n">
-        <v>0.53954802259887</v>
+        <v>0.5508474576271186</v>
       </c>
       <c r="V7" t="n">
-        <v>0.2971014492753624</v>
+        <v>0.3297101449275363</v>
       </c>
       <c r="W7" t="n">
-        <v>0.459915611814346</v>
+        <v>0.4261603375527426</v>
       </c>
       <c r="X7" t="n">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.6534653465346535</v>
+        <v>0.6633663366336634</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.1688311688311688</v>
+        <v>0.1894736842105263</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.2363636363636364</v>
+        <v>0.1875</v>
       </c>
       <c r="AC7" t="n">
         <v>0.7004405286343612</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.6824034334763949</v>
+        <v>0.703862660944206</v>
       </c>
       <c r="AE7" t="n">
         <v>0.7951807228915663</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.8024691358024691</v>
+        <v>0.7951807228915663</v>
       </c>
       <c r="AG7" t="n">
+        <v>0.7840909090909091</v>
+      </c>
+      <c r="AH7" t="n">
         <v>0.7727272727272727</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>0.7613636363636364</v>
       </c>
       <c r="AI7" t="n">
         <v>0.7875000000000001</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.788235294117647</v>
+        <v>0.8</v>
       </c>
       <c r="AK7" t="n">
         <v>0</v>
@@ -2117,7 +2117,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7909090909090909</v>
+        <v>0.8363636363636363</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -2132,94 +2132,94 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8578125000000001</v>
+        <v>0.8906752411575563</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9214659685863875</v>
+        <v>0.9361702127659575</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9322916666666666</v>
+        <v>0.9315789473684211</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5135552272727273</v>
+        <v>0.5312109090909092</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5477250709690028</v>
+        <v>0.5525508425193906</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8364318134472984</v>
+        <v>0.8311638711958134</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8257006151742993</v>
+        <v>0.7997265892002733</v>
       </c>
       <c r="N8" t="n">
-        <v>0.290566037735849</v>
+        <v>0.2576923076923077</v>
       </c>
       <c r="O8" t="n">
-        <v>0.3673469387755102</v>
+        <v>0.006679764243614931</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2009569377990431</v>
+        <v>0.1642512077294686</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2765957446808511</v>
+        <v>0.2315789473684211</v>
       </c>
       <c r="R8" t="n">
-        <v>0.7835820895522387</v>
+        <v>0.7910447761194029</v>
       </c>
       <c r="S8" t="n">
-        <v>0.7633136094674556</v>
+        <v>0.7247191011235955</v>
       </c>
       <c r="T8" t="n">
         <v>0.7362637362637363</v>
       </c>
       <c r="U8" t="n">
-        <v>0.6412429378531074</v>
+        <v>0.6440677966101694</v>
       </c>
       <c r="V8" t="n">
-        <v>0.4456521739130435</v>
+        <v>0.4818840579710146</v>
       </c>
       <c r="W8" t="n">
-        <v>0.5780590717299577</v>
+        <v>0.5358649789029535</v>
       </c>
       <c r="X8" t="n">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.7821782178217822</v>
+        <v>0.7920792079207921</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.3376623376623377</v>
+        <v>0.3473684210526315</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.3818181818181818</v>
+        <v>0.296875</v>
       </c>
       <c r="AC8" t="n">
         <v>0.7753303964757708</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.7424892703862661</v>
+        <v>0.7553648068669528</v>
       </c>
       <c r="AE8" t="n">
+        <v>0.8674698795180723</v>
+      </c>
+      <c r="AF8" t="n">
         <v>0.855421686746988</v>
       </c>
-      <c r="AF8" t="n">
-        <v>0.8765432098765431</v>
-      </c>
       <c r="AG8" t="n">
+        <v>0.8522727272727273</v>
+      </c>
+      <c r="AH8" t="n">
         <v>0.8295454545454546</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>0.8181818181818182</v>
       </c>
       <c r="AI8" t="n">
         <v>0.8500000000000001</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.8470588235294118</v>
+        <v>0.8588235294117647</v>
       </c>
       <c r="AK8" t="n">
         <v>1</v>
@@ -2373,10 +2373,10 @@
         <v>0.9999999999999999</v>
       </c>
       <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
         <v>0.9999999999999999</v>
-      </c>
-      <c r="O9" t="n">
-        <v>1</v>
       </c>
       <c r="P9" t="n">
         <v>0.9999999999999999</v>
@@ -2412,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AB9" t="n">
         <v>1</v>

</xml_diff>